<commit_message>
Added better timesheet and screenshot of Plastic SCM
</commit_message>
<xml_diff>
--- a/Assets/Important/Timesheet/Timesheet - Advanced Tools.xlsx
+++ b/Assets/Important/Timesheet/Timesheet - Advanced Tools.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mauri\Unity Projects\Advanced Tools\Assets\Important\Timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5654A9AA-8D0A-4E36-A602-9678E6CF2B79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1121B22-D18B-489A-BC76-A742EB7F2D69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51480" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{9632AE8E-B98F-49FF-90ED-EE2AB8D66D72}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{9632AE8E-B98F-49FF-90ED-EE2AB8D66D72}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -414,10 +414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C973FE52-08B9-4FF5-822B-F6AA480DB505}">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -453,63 +453,63 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
+        <v>44632</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
         <v>44633</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B5" s="2">
         <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>44634</v>
-      </c>
-      <c r="B5" s="2">
-        <v>1.3</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>44640</v>
+        <v>44634</v>
       </c>
       <c r="B6" s="2">
-        <v>1.2</v>
+        <v>1.3</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>44645</v>
-      </c>
-      <c r="B7">
-        <v>1.5</v>
+        <v>44640</v>
+      </c>
+      <c r="B7" s="2">
+        <v>1.2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>44646</v>
-      </c>
-      <c r="B8" s="2">
-        <v>2.2999999999999998</v>
+        <v>44644</v>
+      </c>
+      <c r="B8">
+        <v>1.5</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
+        <v>44646</v>
+      </c>
+      <c r="B9" s="2">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
         <v>44647</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B10" s="2">
         <v>1.7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
-        <v>44653</v>
-      </c>
-      <c r="B10">
-        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
-        <v>44654</v>
+        <v>44653</v>
       </c>
       <c r="B11">
         <v>5</v>
@@ -517,43 +517,51 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
-        <v>44655</v>
+        <v>44654</v>
       </c>
       <c r="B12">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
-        <v>44667</v>
+        <v>44655</v>
       </c>
       <c r="B13">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
-        <v>44668</v>
+        <v>44660</v>
       </c>
       <c r="B14">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
-        <v>44669</v>
+        <v>44661</v>
       </c>
       <c r="B15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="5">
+        <v>44662</v>
+      </c>
+      <c r="B16">
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B16">
-        <f xml:space="preserve"> SUM(B2:B15)</f>
-        <v>53</v>
+      <c r="B17">
+        <f xml:space="preserve"> SUM(B2:B16)</f>
+        <v>53.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>